<commit_message>
accept clinical_trials as priority value in orders
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.25.mip.xlsx
+++ b/tests/fixtures/orderforms/1508.25.mip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092D3567-32C9-FF41-965F-3BA2CB99272E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66172FD0-99D4-DB43-9B37-483854B368E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4651,7 +4651,7 @@
   <dimension ref="A1:AML395"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J56"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -15509,7 +15509,7 @@
         <v>109</v>
       </c>
       <c r="J18" s="104" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="K18" s="158">
         <v>1</v>
@@ -16568,7 +16568,7 @@
         <v>115</v>
       </c>
       <c r="J19" s="104" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K19" s="158">
         <v>1</v>
@@ -17627,7 +17627,7 @@
         <v>155</v>
       </c>
       <c r="J20" s="104" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K20" s="158">
         <v>1</v>
@@ -18686,7 +18686,7 @@
         <v>125</v>
       </c>
       <c r="J21" s="104" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="K21" s="158">
         <v>1</v>

</xml_diff>

<commit_message>
Feat(db): priority as enum (#1352)
### Refactored:
* Make priority into an enum

### Added:
* Add possibility to filter on priority in admin views

### Changed:
* accept clinical_trials as priority value in orders
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.25.mip.xlsx
+++ b/tests/fixtures/orderforms/1508.25.mip.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092D3567-32C9-FF41-965F-3BA2CB99272E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66172FD0-99D4-DB43-9B37-483854B368E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="27840" windowHeight="17500" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4651,7 +4651,7 @@
   <dimension ref="A1:AML395"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J56"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -15509,7 +15509,7 @@
         <v>109</v>
       </c>
       <c r="J18" s="104" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="K18" s="158">
         <v>1</v>
@@ -16568,7 +16568,7 @@
         <v>115</v>
       </c>
       <c r="J19" s="104" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="K19" s="158">
         <v>1</v>
@@ -17627,7 +17627,7 @@
         <v>155</v>
       </c>
       <c r="J20" s="104" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K20" s="158">
         <v>1</v>
@@ -18686,7 +18686,7 @@
         <v>125</v>
       </c>
       <c r="J21" s="104" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="K21" s="158">
         <v>1</v>

</xml_diff>